<commit_message>
Update Worksheets for calculations.xlsx
</commit_message>
<xml_diff>
--- a/statistics/Worksheets for calculations.xlsx
+++ b/statistics/Worksheets for calculations.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandipto.sanyal\OneDrive - Accenture\Documents\Study materials\AMPBA\git repository\ampba\foundation term\ampba\statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandipto.sanyal\OneDrive - Accenture\Documents\Study materials\AMPBA\git repository\ampba\conceptual examples\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627A8DC4-D707-4B0E-B97E-DFDCE8CAB9FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F8E38A-61E9-43B1-AD1C-C1F25B79BE34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cricketer Bayes theorem" sheetId="1" r:id="rId1"/>
+    <sheet name="Covariance" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cricketer Bayes theorem'!$A$1:$I$12</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Smokes</t>
   </si>
@@ -75,6 +76,57 @@
   </si>
   <si>
     <t>P(Not Character | Not Cricketer)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>5.X</t>
+  </si>
+  <si>
+    <t>6.Y</t>
+  </si>
+  <si>
+    <t>E(X)</t>
+  </si>
+  <si>
+    <t>E(Y)</t>
+  </si>
+  <si>
+    <t>E(5.X)</t>
+  </si>
+  <si>
+    <t>E(6.Y)</t>
+  </si>
+  <si>
+    <t>(X - E(X))</t>
+  </si>
+  <si>
+    <t>(Y-E(Y))</t>
+  </si>
+  <si>
+    <t>COV(X,Y)</t>
+  </si>
+  <si>
+    <t>(X-E(X))*(Y-E(Y))</t>
+  </si>
+  <si>
+    <t>(5.X-E(5.X))*(6.Y-E(6.Y))</t>
+  </si>
+  <si>
+    <t>COV(5.X,6.Y)</t>
+  </si>
+  <si>
+    <t>Scaling of Covariances</t>
+  </si>
+  <si>
+    <t>Corr(X,Y)</t>
+  </si>
+  <si>
+    <t>Corr(5.X,6.Y)</t>
   </si>
 </sst>
 </file>
@@ -212,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -242,6 +294,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -798,5 +853,509 @@
     <mergeCell ref="E4:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA93259A-4DDC-4814-BC40-2FEEB34B86DD}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <f ca="1">RANDBETWEEN(5,15)</f>
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <f ca="1">RANDBETWEEN(5,15)</f>
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <f ca="1">5*A2</f>
+        <v>55</v>
+      </c>
+      <c r="D2" s="2">
+        <f ca="1">6*B2</f>
+        <v>66</v>
+      </c>
+      <c r="E2" s="2">
+        <f ca="1">AVERAGE(A$2:A$9)</f>
+        <v>10.625</v>
+      </c>
+      <c r="F2" s="2">
+        <f ca="1">AVERAGE(B$2:B$9)</f>
+        <v>9.375</v>
+      </c>
+      <c r="G2" s="2">
+        <f ca="1">AVERAGE(C$2:C$9)</f>
+        <v>53.125</v>
+      </c>
+      <c r="H2" s="2">
+        <f ca="1">AVERAGE(D$2:D$9)</f>
+        <v>56.25</v>
+      </c>
+      <c r="I2" s="2">
+        <f ca="1">A2-E2</f>
+        <v>0.375</v>
+      </c>
+      <c r="J2" s="2">
+        <f ca="1">B2-F2</f>
+        <v>1.625</v>
+      </c>
+      <c r="K2" s="2">
+        <f ca="1">I2*J2</f>
+        <v>0.609375</v>
+      </c>
+      <c r="L2" s="2">
+        <f ca="1">(C2-G2)*(D2-H2)</f>
+        <v>18.28125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:B9" ca="1" si="0">RANDBETWEEN(5,15)</f>
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">5*A3</f>
+        <v>60</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D9" ca="1" si="1">6*B3</f>
+        <v>66</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:F9" ca="1" si="2">AVERAGE(A$2:A$9)</f>
+        <v>10.625</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G9" ca="1" si="3">AVERAGE(C$2:C$9)</f>
+        <v>53.125</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H9" ca="1" si="4">AVERAGE(D$2:D$9)</f>
+        <v>56.25</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I9" ca="1" si="5">A3-E3</f>
+        <v>1.375</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J9" ca="1" si="6">B3-F3</f>
+        <v>1.625</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K9" ca="1" si="7">I3*J3</f>
+        <v>2.234375</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L9" ca="1" si="8">(C3-G3)*(D3-H3)</f>
+        <v>67.03125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <f ca="1">5*A4</f>
+        <v>70</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.625</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>53.125</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ca="1" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>3.375</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.625</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ca="1" si="7"/>
+        <v>8.859375</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>265.78125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <f ca="1">5*A5</f>
+        <v>60</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.625</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>53.125</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ca="1" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.375</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.375</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" ca="1" si="7"/>
+        <v>-1.890625</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>-56.71875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <f ca="1">5*A6</f>
+        <v>30</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.625</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>53.125</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" ca="1" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>-4.625</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.625</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" ca="1" si="7"/>
+        <v>-12.140625</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>-364.21875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <f ca="1">5*A7</f>
+        <v>35</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.625</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>53.125</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ca="1" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>-3.625</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>-3.375</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ca="1" si="7"/>
+        <v>12.234375</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>367.03125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <f ca="1">5*A8</f>
+        <v>60</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.625</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>53.125</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ca="1" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.375</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>-4.375</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.015625</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>-180.46875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <f ca="1">5*A9</f>
+        <v>55</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.625</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.375</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>53.125</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ca="1" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.375</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.625</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.234375</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>7.03125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2">
+        <f ca="1">AVERAGE(K2:K9)</f>
+        <v>0.515625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2">
+        <f ca="1">AVERAGE(L2:L9)</f>
+        <v>15.46875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2">
+        <f ca="1">B12/B11</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2">
+        <f ca="1">B11/(_xlfn.STDEV.P(A2:A9)*_xlfn.STDEV.P(B2:B9))</f>
+        <v>7.9518072289156638E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2">
+        <f ca="1">B12/(_xlfn.STDEV.P(C2:C9)*_xlfn.STDEV.P(D2:D9))</f>
+        <v>7.9518072289156624E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>